<commit_message>
Registro de tiempos iteración 4
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_4  Registro.xlsx
+++ b/Documentos/Tareas/Iteración_4  Registro.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-REX\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymu\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A7CA38-AF56-47B2-8836-B6A9C047C99E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469B713A-8875-432B-868C-E561A2BC880B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
   <si>
     <t>Columna</t>
   </si>
@@ -808,10 +808,10 @@
   <dimension ref="B1:BA54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AI6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AK13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AX13" sqref="AX13"/>
+      <selection pane="bottomRight" activeCell="AZ30" sqref="AZ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,96 +1110,96 @@
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8">
         <f>G6-H6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8">
         <f t="shared" ref="L6:L26" si="0">I6-K6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8">
         <f t="shared" ref="O6:O26" si="1">L6-N6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
         <f t="shared" ref="R6:R26" si="2">O6-Q6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U26" si="3">R6-T6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X26" si="4">U6-W6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA26" si="5">X6-Z6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD26" si="6">AA6-AC6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG26" si="7">AD6-AF6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ26" si="8">AG6-AI6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM26" si="9">AJ6-AL6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP26" si="10">AM6-AO6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS26" si="11">AP6-AR6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV26" si="12">AS6-AU6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY26" si="13">AV6-AX6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ26" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA26" si="15">G6-AZ6</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:53" x14ac:dyDescent="0.25">
@@ -1221,96 +1221,96 @@
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8">
         <f>G7-H7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8">
         <f t="shared" ref="L7" si="16">I7-K7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8">
         <f t="shared" ref="O7" si="17">L7-N7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" ref="R7" si="18">O7-Q7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" ref="U7" si="19">R7-T7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" ref="X7" si="20">U7-W7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" ref="AA7" si="21">X7-Z7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" ref="AD7" si="22">AA7-AC7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" ref="AG7" si="23">AD7-AF7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" ref="AJ7" si="24">AG7-AI7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" ref="AM7" si="25">AJ7-AL7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" ref="AP7" si="26">AM7-AO7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" ref="AS7" si="27">AP7-AR7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" ref="AV7" si="28">AS7-AU7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" ref="AY7" si="29">AV7-AX7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" ref="AZ7" si="30">H7+K7+N7+Q7+T7+W7+Z7+AC7+AF7+AI7+AL7+AO7+AR7+AU7+AX7</f>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="BA7" s="11">
         <f t="shared" ref="BA7" si="31">G7-AZ7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:53" x14ac:dyDescent="0.25">
@@ -1332,96 +1332,96 @@
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8">
         <f t="shared" ref="I8:I26" si="32">G8-H8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S8" s="10"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:53" x14ac:dyDescent="0.25">
@@ -1449,96 +1449,96 @@
         <v>64</v>
       </c>
       <c r="G9" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8">
         <f>G9-H9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8">
         <f t="shared" ref="L9" si="33">I9-K9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8">
         <f t="shared" ref="O9" si="34">L9-N9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8">
         <f t="shared" ref="R9" si="35">O9-Q9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S9" s="10"/>
       <c r="T9" s="8"/>
       <c r="U9" s="8">
         <f t="shared" ref="U9" si="36">R9-T9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8">
         <f t="shared" ref="X9" si="37">U9-W9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8">
         <f t="shared" ref="AA9" si="38">X9-Z9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB9" s="10"/>
       <c r="AC9" s="8"/>
       <c r="AD9" s="8">
         <f t="shared" ref="AD9" si="39">AA9-AC9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE9" s="10"/>
       <c r="AF9" s="8"/>
       <c r="AG9" s="8">
         <f t="shared" ref="AG9" si="40">AD9-AF9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH9" s="10"/>
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8">
         <f t="shared" ref="AJ9" si="41">AG9-AI9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK9" s="10"/>
       <c r="AL9" s="8"/>
       <c r="AM9" s="8">
         <f t="shared" ref="AM9" si="42">AJ9-AL9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN9" s="10"/>
       <c r="AO9" s="8"/>
       <c r="AP9" s="8">
         <f t="shared" ref="AP9" si="43">AM9-AO9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ9" s="10"/>
       <c r="AR9" s="8"/>
       <c r="AS9" s="8">
         <f t="shared" ref="AS9" si="44">AP9-AR9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT9" s="10"/>
       <c r="AU9" s="8"/>
       <c r="AV9" s="8">
         <f t="shared" ref="AV9" si="45">AS9-AU9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW9" s="10"/>
       <c r="AX9" s="8"/>
       <c r="AY9" s="8">
         <f t="shared" ref="AY9" si="46">AV9-AX9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ9" s="11">
         <f t="shared" ref="AZ9" si="47">H9+K9+N9+Q9+T9+W9+Z9+AC9+AF9+AI9+AL9+AO9+AR9+AU9+AX9</f>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="BA9" s="11">
         <f t="shared" ref="BA9" si="48">G9-AZ9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:53" x14ac:dyDescent="0.25">
@@ -1675,96 +1675,96 @@
         <v>64</v>
       </c>
       <c r="G11" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8">
         <f>G11-H11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8">
         <f t="shared" ref="L11" si="49">I11-K11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8">
         <f t="shared" ref="O11" si="50">L11-N11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8">
         <f t="shared" ref="R11" si="51">O11-Q11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S11" s="10"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8">
         <f t="shared" ref="U11" si="52">R11-T11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V11" s="10"/>
       <c r="W11" s="8"/>
       <c r="X11" s="8">
         <f t="shared" ref="X11" si="53">U11-W11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y11" s="10"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8">
         <f t="shared" ref="AA11" si="54">X11-Z11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB11" s="10"/>
       <c r="AC11" s="8"/>
       <c r="AD11" s="8">
         <f t="shared" ref="AD11" si="55">AA11-AC11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE11" s="10"/>
       <c r="AF11" s="8"/>
       <c r="AG11" s="8">
         <f t="shared" ref="AG11" si="56">AD11-AF11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH11" s="10"/>
       <c r="AI11" s="8"/>
       <c r="AJ11" s="8">
         <f t="shared" ref="AJ11" si="57">AG11-AI11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK11" s="10"/>
       <c r="AL11" s="8"/>
       <c r="AM11" s="8">
         <f t="shared" ref="AM11" si="58">AJ11-AL11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN11" s="10"/>
       <c r="AO11" s="8"/>
       <c r="AP11" s="8">
         <f t="shared" ref="AP11" si="59">AM11-AO11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="8">
         <f t="shared" ref="AS11" si="60">AP11-AR11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT11" s="10"/>
       <c r="AU11" s="8"/>
       <c r="AV11" s="8">
         <f t="shared" ref="AV11" si="61">AS11-AU11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW11" s="10"/>
       <c r="AX11" s="8"/>
       <c r="AY11" s="8">
         <f t="shared" ref="AY11" si="62">AV11-AX11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ11" s="11">
         <f t="shared" ref="AZ11" si="63">H11+K11+N11+Q11+T11+W11+Z11+AC11+AF11+AI11+AL11+AO11+AR11+AU11+AX11</f>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="BA11" s="11">
         <f t="shared" ref="BA11" si="64">G11-AZ11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:53" x14ac:dyDescent="0.25">
@@ -1792,90 +1792,90 @@
         <v>65</v>
       </c>
       <c r="G12" s="14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8">
         <f t="shared" si="32"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="8"/>
       <c r="O12" s="8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="S12" s="10"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V12" s="10"/>
       <c r="W12" s="8"/>
       <c r="X12" s="8">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="Y12" s="10"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="8"/>
       <c r="AG12" s="8">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AK12" s="10"/>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AN12" s="10"/>
       <c r="AO12" s="8"/>
       <c r="AP12" s="8">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AT12" s="10"/>
       <c r="AU12" s="8"/>
       <c r="AV12" s="8">
         <f t="shared" si="12"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AW12" s="10"/>
       <c r="AX12" s="8">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="AY12" s="8">
         <f t="shared" si="13"/>
-        <v>7.5</v>
+        <v>1.5</v>
       </c>
       <c r="AZ12" s="11">
         <f t="shared" si="14"/>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="BA12" s="11">
         <f t="shared" si="15"/>
-        <v>7.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="2:53" x14ac:dyDescent="0.25">
@@ -1907,90 +1907,90 @@
         <v>65</v>
       </c>
       <c r="G13" s="14">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8">
         <f>G13-H13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8">
         <f t="shared" ref="L13" si="65">I13-K13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8">
         <f t="shared" ref="O13" si="66">L13-N13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8">
         <f t="shared" ref="R13" si="67">O13-Q13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="S13" s="10"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8">
         <f t="shared" ref="U13" si="68">R13-T13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="V13" s="10"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8">
         <f t="shared" ref="X13" si="69">U13-W13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8">
         <f t="shared" ref="AA13" si="70">X13-Z13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8">
         <f t="shared" ref="AD13" si="71">AA13-AC13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8">
         <f t="shared" ref="AG13" si="72">AD13-AF13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8">
         <f t="shared" ref="AJ13" si="73">AG13-AI13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" ref="AM13" si="74">AJ13-AL13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" ref="AP13" si="75">AM13-AO13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" ref="AS13" si="76">AP13-AR13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" ref="AV13" si="77">AS13-AU13</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="AY13" s="8">
         <f t="shared" ref="AY13" si="78">AV13-AX13</f>
-        <v>-10</v>
+        <v>-4</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" ref="AZ13" si="79">H13+K13+N13+Q13+T13+W13+Z13+AC13+AF13+AI13+AL13+AO13+AR13+AU13+AX13</f>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="BA13" s="11">
         <f t="shared" ref="BA13" si="80">G13-AZ13</f>
-        <v>-10</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="14" spans="2:53" x14ac:dyDescent="0.25">
@@ -2135,106 +2135,110 @@
       <c r="E15" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="20"/>
+      <c r="F15" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="G15" s="14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8">
         <f>G15-H15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8">
         <f t="shared" ref="L15" si="81">I15-K15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8">
         <f t="shared" ref="O15" si="82">L15-N15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8">
         <f t="shared" ref="R15" si="83">O15-Q15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="S15" s="10"/>
       <c r="T15" s="8"/>
       <c r="U15" s="8">
         <f t="shared" ref="U15" si="84">R15-T15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="V15" s="10"/>
       <c r="W15" s="8"/>
       <c r="X15" s="8">
         <f t="shared" ref="X15" si="85">U15-W15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="10"/>
       <c r="Z15" s="8"/>
       <c r="AA15" s="8">
         <f t="shared" ref="AA15" si="86">X15-Z15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AB15" s="10"/>
       <c r="AC15" s="8"/>
       <c r="AD15" s="8">
         <f t="shared" ref="AD15" si="87">AA15-AC15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AE15" s="10"/>
       <c r="AF15" s="8"/>
       <c r="AG15" s="8">
         <f t="shared" ref="AG15" si="88">AD15-AF15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AH15" s="10"/>
       <c r="AI15" s="8"/>
       <c r="AJ15" s="8">
         <f t="shared" ref="AJ15" si="89">AG15-AI15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AK15" s="10"/>
       <c r="AL15" s="8"/>
       <c r="AM15" s="8">
         <f t="shared" ref="AM15" si="90">AJ15-AL15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AN15" s="10"/>
       <c r="AO15" s="8"/>
       <c r="AP15" s="8">
         <f t="shared" ref="AP15" si="91">AM15-AO15</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AQ15" s="10"/>
-      <c r="AR15" s="8"/>
+      <c r="AR15" s="8">
+        <v>1</v>
+      </c>
       <c r="AS15" s="8">
         <f t="shared" ref="AS15" si="92">AP15-AR15</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AT15" s="10"/>
       <c r="AU15" s="8"/>
       <c r="AV15" s="8">
         <f t="shared" ref="AV15" si="93">AS15-AU15</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AW15" s="10"/>
       <c r="AX15" s="8"/>
       <c r="AY15" s="8">
         <f t="shared" ref="AY15" si="94">AV15-AX15</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AZ15" s="11">
         <f t="shared" ref="AZ15" si="95">H15+K15+N15+Q15+T15+W15+Z15+AC15+AF15+AI15+AL15+AO15+AR15+AU15+AX15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA15" s="11">
         <f t="shared" ref="BA15" si="96">G15-AZ15</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:53" x14ac:dyDescent="0.25">
@@ -2246,106 +2250,112 @@
       <c r="E16" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="20"/>
+      <c r="F16" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="G16" s="14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8">
         <f t="shared" si="32"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S16" s="10"/>
       <c r="T16" s="8"/>
       <c r="U16" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="V16" s="10"/>
       <c r="W16" s="8"/>
       <c r="X16" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Y16" s="10"/>
       <c r="Z16" s="8"/>
       <c r="AA16" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AB16" s="10"/>
       <c r="AC16" s="8"/>
       <c r="AD16" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AE16" s="10"/>
       <c r="AF16" s="8"/>
       <c r="AG16" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AH16" s="10"/>
-      <c r="AI16" s="8"/>
+      <c r="AI16" s="8">
+        <v>2</v>
+      </c>
       <c r="AJ16" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK16" s="10"/>
       <c r="AL16" s="8"/>
       <c r="AM16" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN16" s="10"/>
-      <c r="AO16" s="8"/>
+      <c r="AO16" s="8">
+        <v>4</v>
+      </c>
       <c r="AP16" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="8"/>
       <c r="AS16" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT16" s="10"/>
       <c r="AU16" s="8"/>
       <c r="AV16" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW16" s="10"/>
       <c r="AX16" s="8"/>
       <c r="AY16" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ16" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BA16" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:53" x14ac:dyDescent="0.25">
@@ -2357,106 +2367,112 @@
       <c r="E17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="20"/>
+      <c r="F17" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="G17" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8">
         <f>G17-H17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8">
         <f t="shared" ref="L17" si="97">I17-K17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8">
         <f t="shared" ref="O17" si="98">L17-N17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8">
         <f t="shared" ref="R17" si="99">O17-Q17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S17" s="10"/>
       <c r="T17" s="8"/>
       <c r="U17" s="8">
         <f t="shared" ref="U17" si="100">R17-T17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V17" s="10"/>
       <c r="W17" s="8"/>
       <c r="X17" s="8">
         <f t="shared" ref="X17" si="101">U17-W17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="8"/>
       <c r="AA17" s="8">
         <f t="shared" ref="AA17" si="102">X17-Z17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB17" s="10"/>
       <c r="AC17" s="8"/>
       <c r="AD17" s="8">
         <f t="shared" ref="AD17" si="103">AA17-AC17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE17" s="10"/>
-      <c r="AF17" s="8"/>
+      <c r="AF17" s="8">
+        <v>0.5</v>
+      </c>
       <c r="AG17" s="8">
         <f t="shared" ref="AG17" si="104">AD17-AF17</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AH17" s="10"/>
       <c r="AI17" s="8"/>
       <c r="AJ17" s="8">
         <f t="shared" ref="AJ17" si="105">AG17-AI17</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AK17" s="10"/>
       <c r="AL17" s="8"/>
       <c r="AM17" s="8">
         <f t="shared" ref="AM17" si="106">AJ17-AL17</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AN17" s="10"/>
       <c r="AO17" s="8"/>
       <c r="AP17" s="8">
         <f t="shared" ref="AP17" si="107">AM17-AO17</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AQ17" s="10"/>
-      <c r="AR17" s="8"/>
+      <c r="AR17" s="8">
+        <v>2</v>
+      </c>
       <c r="AS17" s="8">
         <f t="shared" ref="AS17" si="108">AP17-AR17</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AT17" s="10"/>
       <c r="AU17" s="8"/>
       <c r="AV17" s="8">
         <f t="shared" ref="AV17" si="109">AS17-AU17</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AW17" s="10"/>
       <c r="AX17" s="8"/>
       <c r="AY17" s="8">
         <f t="shared" ref="AY17" si="110">AV17-AX17</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AZ17" s="11">
         <f t="shared" ref="AZ17" si="111">H17+K17+N17+Q17+T17+W17+Z17+AC17+AF17+AI17+AL17+AO17+AR17+AU17+AX17</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="BA17" s="11">
         <f t="shared" ref="BA17" si="112">G17-AZ17</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="18" spans="2:53" x14ac:dyDescent="0.25">
@@ -2474,96 +2490,96 @@
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8">
         <f t="shared" si="32"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S18" s="10"/>
       <c r="T18" s="8"/>
       <c r="U18" s="8">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="V18" s="10"/>
       <c r="W18" s="8"/>
       <c r="X18" s="8">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Y18" s="10"/>
       <c r="Z18" s="8"/>
       <c r="AA18" s="8">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB18" s="10"/>
       <c r="AC18" s="8"/>
       <c r="AD18" s="8">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AE18" s="10"/>
       <c r="AF18" s="8"/>
       <c r="AG18" s="8">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AH18" s="10"/>
       <c r="AI18" s="8"/>
       <c r="AJ18" s="8">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AK18" s="10"/>
       <c r="AL18" s="8"/>
       <c r="AM18" s="8">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AN18" s="10"/>
       <c r="AO18" s="8"/>
       <c r="AP18" s="8">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="8"/>
       <c r="AS18" s="8">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AT18" s="10"/>
       <c r="AU18" s="8"/>
       <c r="AV18" s="8">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AW18" s="10"/>
       <c r="AX18" s="8"/>
       <c r="AY18" s="8">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AZ18" s="11">
         <f t="shared" si="14"/>
@@ -2571,7 +2587,7 @@
       </c>
       <c r="BA18" s="11">
         <f t="shared" si="15"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:53" x14ac:dyDescent="0.25">
@@ -2585,96 +2601,96 @@
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8">
         <f>G19-H19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8">
         <f t="shared" ref="L19" si="113">I19-K19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8">
         <f t="shared" ref="O19" si="114">L19-N19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8">
         <f t="shared" ref="R19" si="115">O19-Q19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S19" s="10"/>
       <c r="T19" s="8"/>
       <c r="U19" s="8">
         <f t="shared" ref="U19" si="116">R19-T19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V19" s="10"/>
       <c r="W19" s="8"/>
       <c r="X19" s="8">
         <f t="shared" ref="X19" si="117">U19-W19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Y19" s="10"/>
       <c r="Z19" s="8"/>
       <c r="AA19" s="8">
         <f t="shared" ref="AA19" si="118">X19-Z19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AB19" s="10"/>
       <c r="AC19" s="8"/>
       <c r="AD19" s="8">
         <f t="shared" ref="AD19" si="119">AA19-AC19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AE19" s="10"/>
       <c r="AF19" s="8"/>
       <c r="AG19" s="8">
         <f t="shared" ref="AG19" si="120">AD19-AF19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AH19" s="10"/>
       <c r="AI19" s="8"/>
       <c r="AJ19" s="8">
         <f t="shared" ref="AJ19" si="121">AG19-AI19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AK19" s="10"/>
       <c r="AL19" s="8"/>
       <c r="AM19" s="8">
         <f t="shared" ref="AM19" si="122">AJ19-AL19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AN19" s="10"/>
       <c r="AO19" s="8"/>
       <c r="AP19" s="8">
         <f t="shared" ref="AP19" si="123">AM19-AO19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AQ19" s="10"/>
       <c r="AR19" s="8"/>
       <c r="AS19" s="8">
         <f t="shared" ref="AS19" si="124">AP19-AR19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AT19" s="10"/>
       <c r="AU19" s="8"/>
       <c r="AV19" s="8">
         <f t="shared" ref="AV19" si="125">AS19-AU19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AW19" s="10"/>
       <c r="AX19" s="8"/>
       <c r="AY19" s="8">
         <f t="shared" ref="AY19" si="126">AV19-AX19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AZ19" s="11">
         <f t="shared" ref="AZ19" si="127">H19+K19+N19+Q19+T19+W19+Z19+AC19+AF19+AI19+AL19+AO19+AR19+AU19+AX19</f>
@@ -2682,7 +2698,7 @@
       </c>
       <c r="BA19" s="11">
         <f t="shared" ref="BA19" si="128">G19-AZ19</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:53" x14ac:dyDescent="0.25">
@@ -2696,96 +2712,96 @@
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S20" s="10"/>
       <c r="T20" s="8"/>
       <c r="U20" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V20" s="10"/>
       <c r="W20" s="8"/>
       <c r="X20" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y20" s="10"/>
       <c r="Z20" s="8"/>
       <c r="AA20" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB20" s="10"/>
       <c r="AC20" s="8"/>
       <c r="AD20" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE20" s="10"/>
       <c r="AF20" s="8"/>
       <c r="AG20" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH20" s="10"/>
       <c r="AI20" s="8"/>
       <c r="AJ20" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK20" s="10"/>
       <c r="AL20" s="8"/>
       <c r="AM20" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN20" s="10"/>
       <c r="AO20" s="8"/>
       <c r="AP20" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ20" s="10"/>
       <c r="AR20" s="8"/>
       <c r="AS20" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT20" s="10"/>
       <c r="AU20" s="8"/>
       <c r="AV20" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW20" s="10"/>
       <c r="AX20" s="8"/>
       <c r="AY20" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ20" s="11">
         <f t="shared" si="14"/>
@@ -2793,7 +2809,7 @@
       </c>
       <c r="BA20" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:53" x14ac:dyDescent="0.25">
@@ -2809,106 +2825,110 @@
       <c r="E21" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="20"/>
+      <c r="F21" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="G21" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8">
         <f>G21-H21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8">
         <f t="shared" ref="L21" si="129">I21-K21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8">
         <f t="shared" ref="O21" si="130">L21-N21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8">
         <f t="shared" ref="R21" si="131">O21-Q21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S21" s="10"/>
       <c r="T21" s="8"/>
       <c r="U21" s="8">
         <f t="shared" ref="U21" si="132">R21-T21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V21" s="10"/>
       <c r="W21" s="8"/>
       <c r="X21" s="8">
         <f t="shared" ref="X21" si="133">U21-W21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="8"/>
       <c r="AA21" s="8">
         <f t="shared" ref="AA21" si="134">X21-Z21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB21" s="10"/>
       <c r="AC21" s="8"/>
       <c r="AD21" s="8">
         <f t="shared" ref="AD21" si="135">AA21-AC21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AE21" s="10"/>
       <c r="AF21" s="8"/>
       <c r="AG21" s="8">
         <f t="shared" ref="AG21" si="136">AD21-AF21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH21" s="10"/>
       <c r="AI21" s="8"/>
       <c r="AJ21" s="8">
         <f t="shared" ref="AJ21" si="137">AG21-AI21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK21" s="10"/>
       <c r="AL21" s="8"/>
       <c r="AM21" s="8">
         <f t="shared" ref="AM21" si="138">AJ21-AL21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN21" s="10"/>
       <c r="AO21" s="8"/>
       <c r="AP21" s="8">
         <f t="shared" ref="AP21" si="139">AM21-AO21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AQ21" s="10"/>
       <c r="AR21" s="8"/>
       <c r="AS21" s="8">
         <f t="shared" ref="AS21" si="140">AP21-AR21</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT21" s="10"/>
-      <c r="AU21" s="8"/>
+      <c r="AU21" s="8">
+        <v>1</v>
+      </c>
       <c r="AV21" s="8">
         <f t="shared" ref="AV21" si="141">AS21-AU21</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AW21" s="10"/>
       <c r="AX21" s="8"/>
       <c r="AY21" s="8">
         <f t="shared" ref="AY21" si="142">AV21-AX21</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AZ21" s="11">
         <f t="shared" ref="AZ21" si="143">H21+K21+N21+Q21+T21+W21+Z21+AC21+AF21+AI21+AL21+AO21+AR21+AU21+AX21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA21" s="11">
         <f t="shared" ref="BA21" si="144">G21-AZ21</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:53" x14ac:dyDescent="0.25">
@@ -2920,106 +2940,110 @@
       <c r="E22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="20"/>
+      <c r="F22" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="G22" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8">
         <f t="shared" si="32"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S22" s="10"/>
       <c r="T22" s="8"/>
       <c r="U22" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V22" s="10"/>
       <c r="W22" s="8"/>
       <c r="X22" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y22" s="10"/>
       <c r="Z22" s="8"/>
       <c r="AA22" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB22" s="10"/>
       <c r="AC22" s="8"/>
       <c r="AD22" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE22" s="10"/>
       <c r="AF22" s="8"/>
       <c r="AG22" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH22" s="10"/>
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK22" s="10"/>
       <c r="AL22" s="8"/>
       <c r="AM22" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN22" s="10"/>
       <c r="AO22" s="8"/>
       <c r="AP22" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AQ22" s="10"/>
       <c r="AR22" s="8"/>
       <c r="AS22" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AT22" s="10"/>
-      <c r="AU22" s="8"/>
+      <c r="AU22" s="8">
+        <v>4</v>
+      </c>
       <c r="AV22" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW22" s="10"/>
       <c r="AX22" s="8"/>
       <c r="AY22" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ22" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA22" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:53" x14ac:dyDescent="0.25">
@@ -3031,106 +3055,110 @@
       <c r="E23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="20"/>
+      <c r="F23" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="G23" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8">
         <f>G23-H23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8">
         <f t="shared" ref="L23" si="145">I23-K23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8">
         <f t="shared" ref="O23" si="146">L23-N23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8">
         <f t="shared" ref="R23" si="147">O23-Q23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S23" s="10"/>
       <c r="T23" s="8"/>
       <c r="U23" s="8">
         <f t="shared" ref="U23" si="148">R23-T23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V23" s="10"/>
       <c r="W23" s="8"/>
       <c r="X23" s="8">
         <f t="shared" ref="X23" si="149">U23-W23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="8"/>
       <c r="AA23" s="8">
         <f t="shared" ref="AA23" si="150">X23-Z23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB23" s="10"/>
       <c r="AC23" s="8"/>
       <c r="AD23" s="8">
         <f t="shared" ref="AD23" si="151">AA23-AC23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE23" s="10"/>
       <c r="AF23" s="8"/>
       <c r="AG23" s="8">
         <f t="shared" ref="AG23" si="152">AD23-AF23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH23" s="10"/>
       <c r="AI23" s="8"/>
       <c r="AJ23" s="8">
         <f t="shared" ref="AJ23" si="153">AG23-AI23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK23" s="10"/>
       <c r="AL23" s="8"/>
       <c r="AM23" s="8">
         <f t="shared" ref="AM23" si="154">AJ23-AL23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN23" s="10"/>
       <c r="AO23" s="8"/>
       <c r="AP23" s="8">
         <f t="shared" ref="AP23" si="155">AM23-AO23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ23" s="10"/>
       <c r="AR23" s="8"/>
       <c r="AS23" s="8">
         <f t="shared" ref="AS23" si="156">AP23-AR23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT23" s="10"/>
-      <c r="AU23" s="8"/>
+      <c r="AU23" s="8">
+        <v>0.5</v>
+      </c>
       <c r="AV23" s="8">
         <f t="shared" ref="AV23" si="157">AS23-AU23</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AW23" s="10"/>
       <c r="AX23" s="8"/>
       <c r="AY23" s="8">
         <f t="shared" ref="AY23" si="158">AV23-AX23</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AZ23" s="11">
         <f t="shared" ref="AZ23" si="159">H23+K23+N23+Q23+T23+W23+Z23+AC23+AF23+AI23+AL23+AO23+AR23+AU23+AX23</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA23" s="11">
         <f t="shared" ref="BA23" si="160">G23-AZ23</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="24" spans="2:53" x14ac:dyDescent="0.25">
@@ -3148,96 +3176,96 @@
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8">
         <f t="shared" si="32"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S24" s="10"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V24" s="10"/>
       <c r="W24" s="8"/>
       <c r="X24" s="8">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="8"/>
       <c r="AA24" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB24" s="10"/>
       <c r="AC24" s="8"/>
       <c r="AD24" s="8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AE24" s="10"/>
       <c r="AF24" s="8"/>
       <c r="AG24" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH24" s="10"/>
       <c r="AI24" s="8"/>
       <c r="AJ24" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK24" s="10"/>
       <c r="AL24" s="8"/>
       <c r="AM24" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN24" s="10"/>
       <c r="AO24" s="8"/>
       <c r="AP24" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AQ24" s="10"/>
       <c r="AR24" s="8"/>
       <c r="AS24" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT24" s="10"/>
       <c r="AU24" s="8"/>
       <c r="AV24" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AW24" s="10"/>
       <c r="AX24" s="8"/>
       <c r="AY24" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AZ24" s="11">
         <f t="shared" si="14"/>
@@ -3245,7 +3273,7 @@
       </c>
       <c r="BA24" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:53" x14ac:dyDescent="0.25">
@@ -3259,96 +3287,96 @@
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="8">
         <f>G25-H25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8">
         <f t="shared" ref="L25" si="161">I25-K25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8">
         <f t="shared" ref="O25" si="162">L25-N25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8">
         <f t="shared" ref="R25" si="163">O25-Q25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S25" s="10"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8">
         <f t="shared" ref="U25" si="164">R25-T25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V25" s="10"/>
       <c r="W25" s="8"/>
       <c r="X25" s="8">
         <f t="shared" ref="X25" si="165">U25-W25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y25" s="10"/>
       <c r="Z25" s="8"/>
       <c r="AA25" s="8">
         <f t="shared" ref="AA25" si="166">X25-Z25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB25" s="10"/>
       <c r="AC25" s="8"/>
       <c r="AD25" s="8">
         <f t="shared" ref="AD25" si="167">AA25-AC25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE25" s="10"/>
       <c r="AF25" s="8"/>
       <c r="AG25" s="8">
         <f t="shared" ref="AG25" si="168">AD25-AF25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH25" s="10"/>
       <c r="AI25" s="8"/>
       <c r="AJ25" s="8">
         <f t="shared" ref="AJ25" si="169">AG25-AI25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK25" s="10"/>
       <c r="AL25" s="8"/>
       <c r="AM25" s="8">
         <f t="shared" ref="AM25" si="170">AJ25-AL25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN25" s="10"/>
       <c r="AO25" s="8"/>
       <c r="AP25" s="8">
         <f t="shared" ref="AP25" si="171">AM25-AO25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AQ25" s="10"/>
       <c r="AR25" s="8"/>
       <c r="AS25" s="8">
         <f t="shared" ref="AS25" si="172">AP25-AR25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AT25" s="10"/>
       <c r="AU25" s="8"/>
       <c r="AV25" s="8">
         <f t="shared" ref="AV25" si="173">AS25-AU25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AW25" s="10"/>
       <c r="AX25" s="8"/>
       <c r="AY25" s="8">
         <f t="shared" ref="AY25" si="174">AV25-AX25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AZ25" s="11">
         <f t="shared" ref="AZ25" si="175">H25+K25+N25+Q25+T25+W25+Z25+AC25+AF25+AI25+AL25+AO25+AR25+AU25+AX25</f>
@@ -3356,7 +3384,7 @@
       </c>
       <c r="BA25" s="11">
         <f t="shared" ref="BA25" si="176">G25-AZ25</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:53" x14ac:dyDescent="0.25">
@@ -3370,96 +3398,96 @@
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="8">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="8"/>
       <c r="R26" s="8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S26" s="10"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V26" s="10"/>
       <c r="W26" s="8"/>
       <c r="X26" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y26" s="10"/>
       <c r="Z26" s="8"/>
       <c r="AA26" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB26" s="10"/>
       <c r="AC26" s="8"/>
       <c r="AD26" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE26" s="10"/>
       <c r="AF26" s="8"/>
       <c r="AG26" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH26" s="10"/>
       <c r="AI26" s="8"/>
       <c r="AJ26" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK26" s="10"/>
       <c r="AL26" s="8"/>
       <c r="AM26" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN26" s="10"/>
       <c r="AO26" s="8"/>
       <c r="AP26" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ26" s="10"/>
       <c r="AR26" s="8"/>
       <c r="AS26" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT26" s="10"/>
       <c r="AU26" s="8"/>
       <c r="AV26" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW26" s="10"/>
       <c r="AX26" s="8"/>
       <c r="AY26" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ26" s="11">
         <f t="shared" si="14"/>
@@ -3467,7 +3495,7 @@
       </c>
       <c r="BA26" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:53" x14ac:dyDescent="0.25">
@@ -6379,11 +6407,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -6395,6 +6418,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Plan de Prueba CU 24 y CU 14- Registro de tareas de la iteración
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_4  Registro.xlsx
+++ b/Documentos/Tareas/Iteración_4  Registro.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymu\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Documents\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469B713A-8875-432B-868C-E561A2BC880B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF633FBF-7E4E-42A4-8631-CC2452503F52}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="66">
   <si>
     <t>Columna</t>
   </si>
@@ -235,7 +235,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +261,14 @@
     <font>
       <b/>
       <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -406,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -472,6 +480,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,10 +822,10 @@
   <dimension ref="B1:BA54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AK13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AI15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AZ30" sqref="AZ30"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1122,9 @@
       <c r="E6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="18" t="s">
+        <v>64</v>
+      </c>
       <c r="G6" s="14">
         <v>1</v>
       </c>
@@ -1219,7 +1235,9 @@
       <c r="E7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>64</v>
+      </c>
       <c r="G7" s="14">
         <v>4</v>
       </c>
@@ -1330,7 +1348,9 @@
       <c r="E8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="18" t="s">
+        <v>64</v>
+      </c>
       <c r="G8" s="14">
         <v>2</v>
       </c>
@@ -2488,7 +2508,9 @@
       <c r="E18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="G18" s="14">
         <v>1</v>
       </c>
@@ -2576,18 +2598,20 @@
         <v>1</v>
       </c>
       <c r="AW18" s="10"/>
-      <c r="AX18" s="8"/>
+      <c r="AX18" s="8">
+        <v>0.5</v>
+      </c>
       <c r="AY18" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ18" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA18" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="2:53" x14ac:dyDescent="0.25">
@@ -2599,7 +2623,9 @@
       <c r="E19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="26" t="s">
+        <v>64</v>
+      </c>
       <c r="G19" s="14">
         <v>5</v>
       </c>
@@ -2710,7 +2736,9 @@
       <c r="E20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="18" t="s">
+        <v>64</v>
+      </c>
       <c r="G20" s="14">
         <v>2</v>
       </c>
@@ -3174,7 +3202,9 @@
       <c r="E24" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="18"/>
+      <c r="F24" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="G24" s="14">
         <v>1</v>
       </c>
@@ -3256,24 +3286,26 @@
         <v>1</v>
       </c>
       <c r="AT24" s="10"/>
-      <c r="AU24" s="8"/>
+      <c r="AU24" s="8">
+        <v>0.5</v>
+      </c>
       <c r="AV24" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW24" s="10"/>
       <c r="AX24" s="8"/>
       <c r="AY24" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ24" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA24" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="2:53" x14ac:dyDescent="0.25">
@@ -3285,7 +3317,9 @@
       <c r="E25" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="F25" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="G25" s="14">
         <v>4</v>
       </c>
@@ -3361,30 +3395,32 @@
         <v>4</v>
       </c>
       <c r="AQ25" s="10"/>
-      <c r="AR25" s="8"/>
+      <c r="AR25" s="8">
+        <v>3</v>
+      </c>
       <c r="AS25" s="8">
         <f t="shared" ref="AS25" si="172">AP25-AR25</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT25" s="10"/>
       <c r="AU25" s="8"/>
       <c r="AV25" s="8">
         <f t="shared" ref="AV25" si="173">AS25-AU25</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AW25" s="10"/>
       <c r="AX25" s="8"/>
       <c r="AY25" s="8">
         <f t="shared" ref="AY25" si="174">AV25-AX25</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AZ25" s="11">
         <f t="shared" ref="AZ25" si="175">H25+K25+N25+Q25+T25+W25+Z25+AC25+AF25+AI25+AL25+AO25+AR25+AU25+AX25</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA25" s="11">
         <f t="shared" ref="BA25" si="176">G25-AZ25</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:53" x14ac:dyDescent="0.25">
@@ -3396,7 +3432,9 @@
       <c r="E26" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="F26" s="18" t="s">
+        <v>64</v>
+      </c>
       <c r="G26" s="14">
         <v>2</v>
       </c>
@@ -3612,7 +3650,9 @@
       <c r="E28" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="18"/>
+      <c r="F28" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="G28" s="14">
         <v>4</v>
       </c>
@@ -3658,60 +3698,66 @@
         <v>4</v>
       </c>
       <c r="AB28" s="10"/>
-      <c r="AC28" s="8"/>
+      <c r="AC28" s="8">
+        <v>1</v>
+      </c>
       <c r="AD28" s="8">
         <f t="shared" si="183"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE28" s="10"/>
       <c r="AF28" s="8"/>
       <c r="AG28" s="8">
         <f t="shared" si="184"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH28" s="10"/>
-      <c r="AI28" s="8"/>
+      <c r="AI28" s="8">
+        <v>2</v>
+      </c>
       <c r="AJ28" s="8">
         <f t="shared" si="185"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK28" s="10"/>
       <c r="AL28" s="8"/>
       <c r="AM28" s="8">
         <f t="shared" si="186"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN28" s="10"/>
-      <c r="AO28" s="8"/>
+      <c r="AO28" s="8">
+        <v>4</v>
+      </c>
       <c r="AP28" s="8">
         <f t="shared" si="187"/>
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="AQ28" s="10"/>
       <c r="AR28" s="8"/>
       <c r="AS28" s="8">
         <f t="shared" si="188"/>
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="AT28" s="10"/>
       <c r="AU28" s="8"/>
       <c r="AV28" s="8">
         <f t="shared" si="189"/>
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="AW28" s="10"/>
       <c r="AX28" s="8"/>
       <c r="AY28" s="8">
         <f t="shared" si="190"/>
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="AZ28" s="11">
         <f t="shared" si="191"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BA28" s="11">
         <f t="shared" si="192"/>
-        <v>4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="29" spans="2:53" x14ac:dyDescent="0.25">
@@ -3904,30 +3950,36 @@
         <v>1</v>
       </c>
       <c r="AQ30" s="10"/>
-      <c r="AR30" s="8"/>
+      <c r="AR30" s="8">
+        <v>0.3</v>
+      </c>
       <c r="AS30" s="8">
         <f t="shared" ref="AS30:AS31" si="204">AP30-AR30</f>
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="AT30" s="10"/>
-      <c r="AU30" s="8"/>
+      <c r="AU30" s="8">
+        <v>0.2</v>
+      </c>
       <c r="AV30" s="8">
         <f t="shared" ref="AV30:AV31" si="205">AS30-AU30</f>
-        <v>1</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="AW30" s="10"/>
-      <c r="AX30" s="8"/>
+      <c r="AX30" s="8">
+        <v>0.3</v>
+      </c>
       <c r="AY30" s="8">
         <f t="shared" ref="AY30:AY31" si="206">AV30-AX30</f>
-        <v>1</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AZ30" s="11">
         <f t="shared" ref="AZ30:AZ31" si="207">H30+K30+N30+Q30+T30+W30+Z30+AC30+AF30+AI30+AL30+AO30+AR30+AU30+AX30</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="BA30" s="11">
         <f t="shared" ref="BA30:BA31" si="208">G30-AZ30</f>
-        <v>1</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="31" spans="2:53" x14ac:dyDescent="0.25">
@@ -3955,90 +4007,92 @@
         <v>1</v>
       </c>
       <c r="M31" s="10"/>
-      <c r="N31" s="8"/>
+      <c r="N31" s="8">
+        <v>1.5</v>
+      </c>
       <c r="O31" s="8">
         <f t="shared" si="194"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="P31" s="10"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8">
         <f t="shared" si="195"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="S31" s="10"/>
       <c r="T31" s="8"/>
       <c r="U31" s="8">
         <f t="shared" si="196"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="V31" s="10"/>
       <c r="W31" s="8"/>
       <c r="X31" s="8">
         <f t="shared" si="197"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="Y31" s="10"/>
       <c r="Z31" s="8"/>
       <c r="AA31" s="8">
         <f t="shared" si="198"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB31" s="10"/>
       <c r="AC31" s="8"/>
       <c r="AD31" s="8">
         <f t="shared" si="199"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AE31" s="10"/>
       <c r="AF31" s="8"/>
       <c r="AG31" s="8">
         <f t="shared" si="200"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AH31" s="10"/>
       <c r="AI31" s="8"/>
       <c r="AJ31" s="8">
         <f t="shared" si="201"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AK31" s="10"/>
       <c r="AL31" s="8"/>
       <c r="AM31" s="8">
         <f t="shared" si="202"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AN31" s="10"/>
       <c r="AO31" s="8"/>
       <c r="AP31" s="8">
         <f t="shared" si="203"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AQ31" s="10"/>
       <c r="AR31" s="8"/>
       <c r="AS31" s="8">
         <f t="shared" si="204"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AT31" s="10"/>
       <c r="AU31" s="8"/>
       <c r="AV31" s="8">
         <f t="shared" si="205"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AW31" s="10"/>
       <c r="AX31" s="8"/>
       <c r="AY31" s="8">
         <f t="shared" si="206"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AZ31" s="11">
         <f t="shared" si="207"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="BA31" s="11">
         <f t="shared" si="208"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="32" spans="2:53" x14ac:dyDescent="0.25">
@@ -4255,7 +4309,7 @@
       <c r="B34" s="13"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="E34" s="27"/>
       <c r="F34" s="5"/>
       <c r="G34" s="14"/>
       <c r="H34" s="8"/>
@@ -6407,6 +6461,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -6418,11 +6477,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>